<commit_message>
add quantiles, code refactor
</commit_message>
<xml_diff>
--- a/src/data/GUS/28 warmińsko-mazurskie.xlsx
+++ b/src/data/GUS/28 warmińsko-mazurskie.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="Ten_skoroszyt" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia\II Stopień (Magister)\Semestr 3\Statystyka w Informatyce\Projekt\chernofffaces\src\data\GUS\New\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia\II Stopień (Magister)\Semestr 3\Statystyka w Informatyce\Projekt\chernofffaces\src\data\GUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="10725" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spis tablic List of tables" sheetId="17" r:id="rId1"/>
@@ -5588,24 +5588,26 @@
   <sheetPr codeName="Arkusz2">
     <tabColor rgb="FF66C2C9"/>
   </sheetPr>
-  <dimension ref="A1:AO340"/>
+  <dimension ref="A1:AQ340"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C317" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="Y8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5:A6"/>
       <selection pane="topRight" activeCell="A5" sqref="A5:A6"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5:A6"/>
-      <selection pane="bottomRight" activeCell="K340" sqref="K340"/>
+      <selection pane="bottomRight" activeCell="AQ9" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="7" customWidth="1"/>
     <col min="3" max="41" width="12.7109375" style="7" customWidth="1"/>
-    <col min="42" max="16384" width="8.85546875" style="7"/>
+    <col min="42" max="42" width="8.85546875" style="7"/>
+    <col min="43" max="43" width="10.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="44" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="76" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="76" customFormat="1" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="125"/>
       <c r="B1" s="125"/>
       <c r="C1" s="73" t="s">
@@ -5650,7 +5652,7 @@
       <c r="AN1" s="75"/>
       <c r="AO1" s="77"/>
     </row>
-    <row r="2" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="128" t="s">
         <v>82</v>
       </c>
@@ -5696,7 +5698,7 @@
       <c r="AN2" s="23"/>
       <c r="AO2" s="24"/>
     </row>
-    <row r="3" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="129" t="s">
         <v>83</v>
       </c>
@@ -5742,7 +5744,7 @@
       <c r="AN3" s="23"/>
       <c r="AO3" s="24"/>
     </row>
-    <row r="4" spans="1:41" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="D4" s="22" t="s">
@@ -5786,7 +5788,7 @@
       <c r="AN4" s="23"/>
       <c r="AO4" s="24"/>
     </row>
-    <row r="5" spans="1:41" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="D5" s="26" t="s">
@@ -5830,7 +5832,7 @@
       <c r="AN5" s="23"/>
       <c r="AO5" s="24"/>
     </row>
-    <row r="6" spans="1:41" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>104</v>
       </c>
@@ -5875,7 +5877,7 @@
       <c r="AN6" s="18"/>
       <c r="AO6" s="25"/>
     </row>
-    <row r="7" spans="1:41" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" ht="22.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
         <v>45</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A8" s="126" t="s">
         <v>47</v>
       </c>
@@ -6124,8 +6126,12 @@
       <c r="AO8" s="70">
         <v>1015502</v>
       </c>
+      <c r="AQ8" s="122">
+        <f>AVERAGE(L8:AO8)</f>
+        <v>1165628.1000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A9" s="126"/>
       <c r="B9" s="9">
         <v>0</v>
@@ -6247,8 +6253,12 @@
       <c r="AO9" s="3">
         <v>6304</v>
       </c>
+      <c r="AQ9" s="122">
+        <f>MEDIAN(L8:AO8)</f>
+        <v>1168060.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A10" s="126"/>
       <c r="B10" s="9">
         <v>1</v>
@@ -6370,8 +6380,12 @@
       <c r="AO10" s="3">
         <v>6505</v>
       </c>
+      <c r="AQ10" s="122">
+        <f>MIN(L8:AO8)</f>
+        <v>1015502</v>
+      </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A11" s="126"/>
       <c r="B11" s="9">
         <v>2</v>
@@ -6493,8 +6507,12 @@
       <c r="AO11" s="3">
         <v>6742</v>
       </c>
+      <c r="AQ11" s="122">
+        <f>MAX(L8:AO8)</f>
+        <v>1305697</v>
+      </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A12" s="126"/>
       <c r="B12" s="9">
         <v>3</v>
@@ -6616,8 +6634,12 @@
       <c r="AO12" s="3">
         <v>6965</v>
       </c>
+      <c r="AQ12" s="7" t="e">
+        <f>PERCENTILE.</f>
+        <v>#NAME?</v>
+      </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A13" s="126"/>
       <c r="B13" s="9">
         <v>4</v>
@@ -6740,7 +6762,7 @@
         <v>7215</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A14" s="126"/>
       <c r="B14" s="9">
         <v>5</v>
@@ -6863,7 +6885,7 @@
         <v>7448</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A15" s="126"/>
       <c r="B15" s="9">
         <v>6</v>
@@ -6986,7 +7008,7 @@
         <v>7672</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A16" s="126"/>
       <c r="B16" s="9">
         <v>7</v>
@@ -7109,7 +7131,7 @@
         <v>7903</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A17" s="126"/>
       <c r="B17" s="9">
         <v>8</v>
@@ -7232,7 +7254,7 @@
         <v>8116</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A18" s="126"/>
       <c r="B18" s="9">
         <v>9</v>
@@ -7355,7 +7377,7 @@
         <v>8329</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A19" s="126"/>
       <c r="B19" s="9">
         <v>10</v>
@@ -7478,7 +7500,7 @@
         <v>8545</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A20" s="126"/>
       <c r="B20" s="9">
         <v>11</v>
@@ -7601,7 +7623,7 @@
         <v>8726</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A21" s="126"/>
       <c r="B21" s="9">
         <v>12</v>
@@ -7724,7 +7746,7 @@
         <v>8905</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A22" s="126"/>
       <c r="B22" s="9">
         <v>13</v>
@@ -7847,7 +7869,7 @@
         <v>9034</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A23" s="126"/>
       <c r="B23" s="9">
         <v>14</v>
@@ -7969,8 +7991,9 @@
       <c r="AO23" s="3">
         <v>9168</v>
       </c>
+      <c r="AQ23" s="122"/>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A24" s="126"/>
       <c r="B24" s="9">
         <v>15</v>
@@ -8093,7 +8116,7 @@
         <v>9257</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A25" s="126"/>
       <c r="B25" s="9">
         <v>16</v>
@@ -8216,7 +8239,7 @@
         <v>9345</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A26" s="126"/>
       <c r="B26" s="9">
         <v>17</v>
@@ -8339,7 +8362,7 @@
         <v>9387</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A27" s="126"/>
       <c r="B27" s="9">
         <v>18</v>
@@ -8462,7 +8485,7 @@
         <v>9415</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A28" s="126"/>
       <c r="B28" s="9">
         <v>19</v>
@@ -8585,7 +8608,7 @@
         <v>9420</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A29" s="126"/>
       <c r="B29" s="9">
         <v>20</v>
@@ -8708,7 +8731,7 @@
         <v>9410</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A30" s="126"/>
       <c r="B30" s="9">
         <v>21</v>
@@ -8831,7 +8854,7 @@
         <v>9381</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A31" s="126"/>
       <c r="B31" s="9">
         <v>22</v>
@@ -8954,7 +8977,7 @@
         <v>9352</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A32" s="126"/>
       <c r="B32" s="9">
         <v>23</v>

</xml_diff>